<commit_message>
added html entities ref
</commit_message>
<xml_diff>
--- a/htaccess.xlsx
+++ b/htaccess.xlsx
@@ -1,16 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10414"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rich/github/clagnut/wbtyp/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23AD6265-76FE-CF4B-8598-23CBA92BBC38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="23800" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -19,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="155">
   <si>
     <t>http://clagnut.com/</t>
   </si>
@@ -481,13 +497,16 @@
   </si>
   <si>
     <t>https://coop-design-manual.herokuapp.com/styles/typography.html</t>
+  </si>
+  <si>
+    <t>https://www.htmlsymbol.com/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -859,12 +878,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="5"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="313">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1183,6 +1201,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1507,18 +1533,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E154"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E155"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A102" workbookViewId="0">
+      <selection activeCell="B156" sqref="B156"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
-    <col min="2" max="2" width="42.375" customWidth="1"/>
-    <col min="3" max="3" width="4.5" customWidth="1"/>
+    <col min="2" max="2" width="42.42578125" customWidth="1"/>
+    <col min="3" max="3" width="4.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -4402,13 +4428,13 @@
       </c>
     </row>
     <row r="145" spans="1:5">
-      <c r="A145" s="4">
+      <c r="A145">
         <v>145</v>
       </c>
       <c r="B145" t="s">
         <v>140</v>
       </c>
-      <c r="C145" s="4" t="str">
+      <c r="C145" t="str">
         <f t="shared" si="15"/>
         <v>&lt;span class='outlink'&gt;(http://wbtyp.net/145)&lt;/span&gt;</v>
       </c>
@@ -4422,13 +4448,13 @@
       </c>
     </row>
     <row r="146" spans="1:5">
-      <c r="A146" s="4">
+      <c r="A146">
         <v>146</v>
       </c>
       <c r="B146" t="s">
         <v>141</v>
       </c>
-      <c r="C146" s="4" t="str">
+      <c r="C146" t="str">
         <f t="shared" si="15"/>
         <v>&lt;span class='outlink'&gt;(http://wbtyp.net/146)&lt;/span&gt;</v>
       </c>
@@ -4442,13 +4468,13 @@
       </c>
     </row>
     <row r="147" spans="1:5">
-      <c r="A147" s="4">
+      <c r="A147">
         <v>147</v>
       </c>
       <c r="B147" t="s">
         <v>142</v>
       </c>
-      <c r="C147" s="4" t="str">
+      <c r="C147" t="str">
         <f t="shared" si="15"/>
         <v>&lt;span class='outlink'&gt;(http://wbtyp.net/147)&lt;/span&gt;</v>
       </c>
@@ -4462,13 +4488,13 @@
       </c>
     </row>
     <row r="148" spans="1:5">
-      <c r="A148" s="4">
+      <c r="A148">
         <v>148</v>
       </c>
       <c r="B148" t="s">
         <v>143</v>
       </c>
-      <c r="C148" s="4" t="str">
+      <c r="C148" t="str">
         <f t="shared" si="15"/>
         <v>&lt;span class='outlink'&gt;(http://wbtyp.net/148)&lt;/span&gt;</v>
       </c>
@@ -4482,13 +4508,13 @@
       </c>
     </row>
     <row r="149" spans="1:5">
-      <c r="A149" s="4">
+      <c r="A149">
         <v>149</v>
       </c>
       <c r="B149" t="s">
         <v>144</v>
       </c>
-      <c r="C149" s="4" t="str">
+      <c r="C149" t="str">
         <f t="shared" si="15"/>
         <v>&lt;span class='outlink'&gt;(http://wbtyp.net/149)&lt;/span&gt;</v>
       </c>
@@ -4502,13 +4528,13 @@
       </c>
     </row>
     <row r="150" spans="1:5">
-      <c r="A150" s="4">
+      <c r="A150">
         <v>150</v>
       </c>
       <c r="B150" t="s">
         <v>145</v>
       </c>
-      <c r="C150" s="4" t="str">
+      <c r="C150" t="str">
         <f t="shared" si="15"/>
         <v>&lt;span class='outlink'&gt;(http://wbtyp.net/150)&lt;/span&gt;</v>
       </c>
@@ -4522,13 +4548,13 @@
       </c>
     </row>
     <row r="151" spans="1:5">
-      <c r="A151" s="4">
+      <c r="A151">
         <v>151</v>
       </c>
       <c r="B151" t="s">
         <v>146</v>
       </c>
-      <c r="C151" s="4" t="str">
+      <c r="C151" t="str">
         <f t="shared" si="15"/>
         <v>&lt;span class='outlink'&gt;(http://wbtyp.net/151)&lt;/span&gt;</v>
       </c>
@@ -4542,13 +4568,13 @@
       </c>
     </row>
     <row r="152" spans="1:5">
-      <c r="A152" s="4">
+      <c r="A152">
         <v>152</v>
       </c>
       <c r="B152" t="s">
         <v>147</v>
       </c>
-      <c r="C152" s="4" t="str">
+      <c r="C152" t="str">
         <f t="shared" si="15"/>
         <v>&lt;span class='outlink'&gt;(http://wbtyp.net/152)&lt;/span&gt;</v>
       </c>
@@ -4562,13 +4588,13 @@
       </c>
     </row>
     <row r="153" spans="1:5">
-      <c r="A153" s="4">
+      <c r="A153">
         <v>153</v>
       </c>
       <c r="B153" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C153" s="4" t="str">
+      <c r="C153" t="str">
         <f t="shared" si="15"/>
         <v>&lt;span class='outlink'&gt;(http://wbtyp.net/153)&lt;/span&gt;</v>
       </c>
@@ -4582,13 +4608,13 @@
       </c>
     </row>
     <row r="154" spans="1:5">
-      <c r="A154" s="4">
+      <c r="A154">
         <v>154</v>
       </c>
       <c r="B154" t="s">
         <v>149</v>
       </c>
-      <c r="C154" s="4" t="str">
+      <c r="C154" t="str">
         <f t="shared" si="15"/>
         <v>&lt;span class='outlink'&gt;(http://wbtyp.net/154)&lt;/span&gt;</v>
       </c>
@@ -4601,15 +4627,36 @@
         <v>&lt;li&gt;http://typedrawers.com&lt;/li&gt;</v>
       </c>
     </row>
+    <row r="155" spans="1:5">
+      <c r="A155">
+        <v>155</v>
+      </c>
+      <c r="B155" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C155" t="str">
+        <f t="shared" ref="C155" si="24">CONCATENATE("&lt;span class='outlink'&gt;(http://wbtyp.net/",A155, ")&lt;/span&gt;")</f>
+        <v>&lt;span class='outlink'&gt;(http://wbtyp.net/155)&lt;/span&gt;</v>
+      </c>
+      <c r="D155" s="3" t="str">
+        <f t="shared" ref="D155" si="25">CONCATENATE("Redirect 301 /",A155," ",B155)</f>
+        <v>Redirect 301 /155 https://www.htmlsymbol.com/</v>
+      </c>
+      <c r="E155" s="3" t="str">
+        <f t="shared" ref="E155" si="26">CONCATENATE("&lt;li&gt;",B155,"&lt;/li&gt;")</f>
+        <v>&lt;li&gt;https://www.htmlsymbol.com/&lt;/li&gt;</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B1" r:id="rId1"/>
-    <hyperlink ref="B4" r:id="rId2"/>
-    <hyperlink ref="B135" r:id="rId3"/>
-    <hyperlink ref="B153" r:id="rId4"/>
-    <hyperlink ref="B30" r:id="rId5"/>
-    <hyperlink ref="B40" r:id="rId6"/>
-    <hyperlink ref="B13" r:id="rId7"/>
+    <hyperlink ref="B1" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B135" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B153" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B30" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B40" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B13" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B155" r:id="rId8" xr:uid="{1A9410C0-94AC-1041-A626-BE9255969806}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>